<commit_message>
Processed EEMs and Saved Pictures
Processed EEMs for Poster and took pictures. 180530
</commit_message>
<xml_diff>
--- a/F3SPF_LOG SHEET_BBWM_180523.xlsx
+++ b/F3SPF_LOG SHEET_BBWM_180523.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="185">
   <si>
     <t>Name of Raw EEM</t>
   </si>
@@ -483,6 +483,102 @@
   </si>
   <si>
     <t>ornl4xc6</t>
+  </si>
+  <si>
+    <t>sjer</t>
+  </si>
+  <si>
+    <t>sjercomb</t>
+  </si>
+  <si>
+    <t>sjercomb, naco3</t>
+  </si>
+  <si>
+    <t>sjercomb, smplhldr</t>
+  </si>
+  <si>
+    <t>sjercomb, naco3, smplhldr</t>
+  </si>
+  <si>
+    <t>sjer5x</t>
+  </si>
+  <si>
+    <t>sjer10x</t>
+  </si>
+  <si>
+    <t>sjer20x</t>
+  </si>
+  <si>
+    <t>sjerc1</t>
+  </si>
+  <si>
+    <t>sjer5xc1</t>
+  </si>
+  <si>
+    <t>sjer10xc1</t>
+  </si>
+  <si>
+    <t>sjer20xc1</t>
+  </si>
+  <si>
+    <t>sjerc2</t>
+  </si>
+  <si>
+    <t>sjerc3</t>
+  </si>
+  <si>
+    <t>sjerc4</t>
+  </si>
+  <si>
+    <t>sjerc5</t>
+  </si>
+  <si>
+    <t>sjerc6</t>
+  </si>
+  <si>
+    <t>sjer5xc2</t>
+  </si>
+  <si>
+    <t>sjer5xc3</t>
+  </si>
+  <si>
+    <t>sjer5xc4</t>
+  </si>
+  <si>
+    <t>sjer5xc5</t>
+  </si>
+  <si>
+    <t>sjer5xc6</t>
+  </si>
+  <si>
+    <t>sjer20xc2</t>
+  </si>
+  <si>
+    <t>sjer10xc2</t>
+  </si>
+  <si>
+    <t>sjer10xc3</t>
+  </si>
+  <si>
+    <t>sjer10xc4</t>
+  </si>
+  <si>
+    <t>sjer10xc5</t>
+  </si>
+  <si>
+    <t>sjer10xc6</t>
+  </si>
+  <si>
+    <t>sjer20xc3</t>
+  </si>
+  <si>
+    <t>sjer20xc4</t>
+  </si>
+  <si>
+    <t>sjer20xc5</t>
+  </si>
+  <si>
+    <t>sjer20xc6</t>
   </si>
 </sst>
 </file>
@@ -834,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="D133" sqref="A110:D133"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110:D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2378,6 +2474,342 @@
         <v>4</v>
       </c>
     </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" t="s">
+        <v>161</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>153</v>
+      </c>
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s">
+        <v>165</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>153</v>
+      </c>
+      <c r="B112" t="s">
+        <v>154</v>
+      </c>
+      <c r="C112" t="s">
+        <v>166</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>153</v>
+      </c>
+      <c r="B113" t="s">
+        <v>156</v>
+      </c>
+      <c r="C113" t="s">
+        <v>167</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>153</v>
+      </c>
+      <c r="B114" t="s">
+        <v>155</v>
+      </c>
+      <c r="C114" t="s">
+        <v>168</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>153</v>
+      </c>
+      <c r="B115" t="s">
+        <v>157</v>
+      </c>
+      <c r="C115" t="s">
+        <v>169</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>158</v>
+      </c>
+      <c r="B116" t="s">
+        <v>11</v>
+      </c>
+      <c r="C116" t="s">
+        <v>162</v>
+      </c>
+      <c r="D116">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>158</v>
+      </c>
+      <c r="B117" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s">
+        <v>170</v>
+      </c>
+      <c r="D117">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>158</v>
+      </c>
+      <c r="B118" t="s">
+        <v>154</v>
+      </c>
+      <c r="C118" t="s">
+        <v>171</v>
+      </c>
+      <c r="D118">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>158</v>
+      </c>
+      <c r="B119" t="s">
+        <v>156</v>
+      </c>
+      <c r="C119" t="s">
+        <v>172</v>
+      </c>
+      <c r="D119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>158</v>
+      </c>
+      <c r="B120" t="s">
+        <v>155</v>
+      </c>
+      <c r="C120" t="s">
+        <v>173</v>
+      </c>
+      <c r="D120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>158</v>
+      </c>
+      <c r="B121" t="s">
+        <v>157</v>
+      </c>
+      <c r="C121" t="s">
+        <v>174</v>
+      </c>
+      <c r="D121">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>159</v>
+      </c>
+      <c r="B122" t="s">
+        <v>11</v>
+      </c>
+      <c r="C122" t="s">
+        <v>163</v>
+      </c>
+      <c r="D122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>159</v>
+      </c>
+      <c r="B123" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s">
+        <v>176</v>
+      </c>
+      <c r="D123">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>159</v>
+      </c>
+      <c r="B124" t="s">
+        <v>154</v>
+      </c>
+      <c r="C124" t="s">
+        <v>177</v>
+      </c>
+      <c r="D124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>159</v>
+      </c>
+      <c r="B125" t="s">
+        <v>156</v>
+      </c>
+      <c r="C125" t="s">
+        <v>178</v>
+      </c>
+      <c r="D125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>159</v>
+      </c>
+      <c r="B126" t="s">
+        <v>155</v>
+      </c>
+      <c r="C126" t="s">
+        <v>179</v>
+      </c>
+      <c r="D126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>159</v>
+      </c>
+      <c r="B127" t="s">
+        <v>157</v>
+      </c>
+      <c r="C127" t="s">
+        <v>180</v>
+      </c>
+      <c r="D127">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>160</v>
+      </c>
+      <c r="B128" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" t="s">
+        <v>164</v>
+      </c>
+      <c r="D128">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>160</v>
+      </c>
+      <c r="B129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s">
+        <v>175</v>
+      </c>
+      <c r="D129">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>160</v>
+      </c>
+      <c r="B130" t="s">
+        <v>154</v>
+      </c>
+      <c r="C130" t="s">
+        <v>181</v>
+      </c>
+      <c r="D130">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>160</v>
+      </c>
+      <c r="B131" t="s">
+        <v>156</v>
+      </c>
+      <c r="C131" t="s">
+        <v>182</v>
+      </c>
+      <c r="D131">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>160</v>
+      </c>
+      <c r="B132" t="s">
+        <v>155</v>
+      </c>
+      <c r="C132" t="s">
+        <v>183</v>
+      </c>
+      <c r="D132">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>160</v>
+      </c>
+      <c r="B133" t="s">
+        <v>157</v>
+      </c>
+      <c r="C133" t="s">
+        <v>184</v>
+      </c>
+      <c r="D133">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>